<commit_message>
Proyecto de sistema de control de cumpleaños
</commit_message>
<xml_diff>
--- a/control-secret/invitados.xlsx
+++ b/control-secret/invitados.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7b6d62b0b7578472/Desktop/juanma/control-secret/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Juanma Viana\Desktop\sistema-control-secret\control-secret\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="215" documentId="8_{9C9106A2-26EC-4318-A9AB-C98922D04795}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DFE8BFF1-18F9-497F-9FFE-2B43CDAAA96D}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9D42BC4-53DE-46BA-BB7A-1E935FA788D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{21B315DA-1669-4AA7-9515-DBF9E548B519}"/>
+    <workbookView xWindow="12816" yWindow="0" windowWidth="10320" windowHeight="12336" xr2:uid="{21B315DA-1669-4AA7-9515-DBF9E548B519}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="181">
   <si>
     <t>Cumpleañero</t>
   </si>
@@ -357,12 +357,255 @@
   <si>
     <t xml:space="preserve">Ezequiel Amarilla </t>
   </si>
+  <si>
+    <t>Julian Pro</t>
+  </si>
+  <si>
+    <t>Maxi Berdum</t>
+  </si>
+  <si>
+    <t>Melisa Kozak</t>
+  </si>
+  <si>
+    <t>Fernando Benítez</t>
+  </si>
+  <si>
+    <t>Franco cañete</t>
+  </si>
+  <si>
+    <t>Ezequiel ramos</t>
+  </si>
+  <si>
+    <t>Juan cueva</t>
+  </si>
+  <si>
+    <t>Facundo cuevas</t>
+  </si>
+  <si>
+    <t>Samara Magali Resquin</t>
+  </si>
+  <si>
+    <t>Thiago Gabriel Gonzalez</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Micaela Leticia Maidana </t>
+  </si>
+  <si>
+    <t>Catalina Victoria Ocampos Kleinbielen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rodrigo Fernández </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Milagros Benítez </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ivana Almeida </t>
+  </si>
+  <si>
+    <t>Benja Rojas</t>
+  </si>
+  <si>
+    <t>Elian Schimpf</t>
+  </si>
+  <si>
+    <t>Gonzalo Talavera</t>
+  </si>
+  <si>
+    <t>Lautaro Gomez</t>
+  </si>
+  <si>
+    <t>Jeremías Reggio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Joaquín Espinoza </t>
+  </si>
+  <si>
+    <t>Ezequiel Giménez</t>
+  </si>
+  <si>
+    <t>Adri drewes</t>
+  </si>
+  <si>
+    <t>Dalila Ayelen Schendelbek</t>
+  </si>
+  <si>
+    <t>Evelin Eliane Martim</t>
+  </si>
+  <si>
+    <t>Selene Marisol Martinez</t>
+  </si>
+  <si>
+    <t>Tobias nicolas mora</t>
+  </si>
+  <si>
+    <t>Belen Villagra</t>
+  </si>
+  <si>
+    <t>Ciara Chaihort</t>
+  </si>
+  <si>
+    <t>Constanza Melgarejo</t>
+  </si>
+  <si>
+    <t>Lourdes Peña</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fredi Alonso </t>
+  </si>
+  <si>
+    <t>Santiago Bottcher</t>
+  </si>
+  <si>
+    <t>Belén Cardozo</t>
+  </si>
+  <si>
+    <t>Angy Rivas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sofía Villalba </t>
+  </si>
+  <si>
+    <t>Matías Rivero</t>
+  </si>
+  <si>
+    <t>villasanti dalma</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Barbonallia Thomas </t>
+  </si>
+  <si>
+    <t>Gonzalez Johansen Leandro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gonzalo riedenauer </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Agustín schapovaloff </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Juan Ángel solis </t>
+  </si>
+  <si>
+    <t>Emiliano arenhardt</t>
+  </si>
+  <si>
+    <t>Miranda Fernando</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lopez Benicio </t>
+  </si>
+  <si>
+    <t>Dos Santos Franco</t>
+  </si>
+  <si>
+    <t>Hinc Facundo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Leonardo fabian Crizante </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Emilia María Antonia jara </t>
+  </si>
+  <si>
+    <t>Ismael José Luis vera</t>
+  </si>
+  <si>
+    <t>Tomas Ernesto Crizante</t>
+  </si>
+  <si>
+    <t>Karen flores</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Angela Camacho </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mirna Camacho </t>
+  </si>
+  <si>
+    <t>Lucas mallorquín</t>
+  </si>
+  <si>
+    <t>Villalba Ornella Giuliana</t>
+  </si>
+  <si>
+    <t>⁠María Victoria Chamorro</t>
+  </si>
+  <si>
+    <t>⁠Ludmila Abril Lopez</t>
+  </si>
+  <si>
+    <t xml:space="preserve">macarena benítez </t>
+  </si>
+  <si>
+    <t>candela gonzález</t>
+  </si>
+  <si>
+    <t>lisandro talavera</t>
+  </si>
+  <si>
+    <t>Flecha Fernanda Ailen</t>
+  </si>
+  <si>
+    <t>Avril Estefanía Acosta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nahiara olivera </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cardozo valentín </t>
+  </si>
+  <si>
+    <t>Talavera nahuel</t>
+  </si>
+  <si>
+    <t>Rodríguez juan</t>
+  </si>
+  <si>
+    <t>Suárez franco</t>
+  </si>
+  <si>
+    <t>Taboada Zaira</t>
+  </si>
+  <si>
+    <t>Brisa Cardozo</t>
+  </si>
+  <si>
+    <t>Vergara Valentina</t>
+  </si>
+  <si>
+    <t>Kukla Camila</t>
+  </si>
+  <si>
+    <t>Garcete Lautaro</t>
+  </si>
+  <si>
+    <t>Lindemann Matías</t>
+  </si>
+  <si>
+    <t>Nuñez Luciana</t>
+  </si>
+  <si>
+    <t>Rodriguez Gonzalo</t>
+  </si>
+  <si>
+    <t>Angel Pellizzer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Agustina cáceres </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fabián Pereyra </t>
+  </si>
+  <si>
+    <t>Simon Duarte</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -382,6 +625,12 @@
       <u/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -437,7 +686,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -753,21 +1002,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D01B39E2-E4E1-4B92-AD5B-ADAFFC13EBEE}">
-  <dimension ref="A1:D145"/>
+  <dimension ref="A1:D144"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A92" workbookViewId="0">
-      <selection activeCell="B113" sqref="B113"/>
+    <sheetView tabSelected="1" topLeftCell="A105" workbookViewId="0">
+      <selection activeCell="B123" sqref="B123"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="31.85546875" customWidth="1"/>
+    <col min="1" max="1" width="31.88671875" customWidth="1"/>
     <col min="2" max="2" width="35" customWidth="1"/>
-    <col min="3" max="3" width="36.28515625" customWidth="1"/>
-    <col min="4" max="4" width="21.85546875" customWidth="1"/>
+    <col min="3" max="3" width="36.33203125" customWidth="1"/>
+    <col min="4" max="4" width="21.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -781,51 +1030,63 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="C2" t="s">
+        <v>148</v>
+      </c>
       <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="C3" t="s">
+        <v>149</v>
+      </c>
       <c r="D3" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="C4" t="s">
+        <v>150</v>
+      </c>
       <c r="D4" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="C5" t="s">
+        <v>151</v>
+      </c>
       <c r="D5" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -839,7 +1100,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
@@ -853,7 +1114,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>10</v>
       </c>
@@ -867,7 +1128,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>10</v>
       </c>
@@ -881,128 +1142,161 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>12</v>
       </c>
       <c r="B10" t="s">
         <v>13</v>
       </c>
+      <c r="C10" t="s">
+        <v>177</v>
+      </c>
       <c r="D10" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>12</v>
       </c>
       <c r="B11" t="s">
         <v>13</v>
       </c>
+      <c r="C11" t="s">
+        <v>178</v>
+      </c>
       <c r="D11" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>12</v>
       </c>
       <c r="B12" t="s">
         <v>13</v>
       </c>
+      <c r="C12" t="s">
+        <v>179</v>
+      </c>
       <c r="D12" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>12</v>
       </c>
       <c r="B13" t="s">
         <v>13</v>
       </c>
+      <c r="C13" t="s">
+        <v>180</v>
+      </c>
       <c r="D13" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>13</v>
+        <v>15</v>
+      </c>
+      <c r="C14" t="s">
+        <v>140</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>14</v>
       </c>
       <c r="B15" t="s">
         <v>15</v>
       </c>
+      <c r="C15" t="s">
+        <v>141</v>
+      </c>
       <c r="D15" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>14</v>
       </c>
       <c r="B16" t="s">
         <v>15</v>
       </c>
+      <c r="C16" t="s">
+        <v>142</v>
+      </c>
       <c r="D16" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>14</v>
       </c>
       <c r="B17" t="s">
         <v>15</v>
       </c>
+      <c r="C17" t="s">
+        <v>143</v>
+      </c>
       <c r="D17" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>15</v>
+        <v>17</v>
+      </c>
+      <c r="C18" t="s">
+        <v>162</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>16</v>
       </c>
       <c r="B19" t="s">
         <v>17</v>
       </c>
+      <c r="C19" t="s">
+        <v>163</v>
+      </c>
       <c r="D19" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>16</v>
       </c>
       <c r="B20" t="s">
         <v>17</v>
       </c>
+      <c r="C20" t="s">
+        <v>164</v>
+      </c>
       <c r="D20" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>16</v>
       </c>
@@ -1013,110 +1307,133 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B22" t="s">
-        <v>17</v>
+        <v>19</v>
+      </c>
+      <c r="C22" t="s">
+        <v>144</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>18</v>
       </c>
       <c r="B23" t="s">
         <v>19</v>
       </c>
+      <c r="C23" t="s">
+        <v>145</v>
+      </c>
       <c r="D23" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>18</v>
       </c>
       <c r="B24" t="s">
         <v>19</v>
       </c>
+      <c r="C24" t="s">
+        <v>146</v>
+      </c>
       <c r="D24" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>18</v>
       </c>
       <c r="B25" t="s">
         <v>19</v>
       </c>
+      <c r="C25" s="2" t="s">
+        <v>147</v>
+      </c>
       <c r="D25" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B26" t="s">
-        <v>19</v>
-      </c>
-      <c r="C26" s="2"/>
+        <v>21</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>100</v>
+      </c>
       <c r="D26" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>20</v>
       </c>
       <c r="B27" t="s">
         <v>21</v>
       </c>
-      <c r="C27" s="2"/>
+      <c r="C27" s="2" t="s">
+        <v>101</v>
+      </c>
       <c r="D27" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>20</v>
       </c>
       <c r="B28" t="s">
         <v>21</v>
       </c>
-      <c r="C28" s="2"/>
+      <c r="C28" s="2" t="s">
+        <v>102</v>
+      </c>
       <c r="D28" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>20</v>
       </c>
       <c r="B29" t="s">
         <v>21</v>
       </c>
-      <c r="C29" s="2"/>
+      <c r="C29" t="s">
+        <v>103</v>
+      </c>
       <c r="D29" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B30" t="s">
-        <v>21</v>
+        <v>23</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>80</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>22</v>
       </c>
@@ -1124,13 +1441,13 @@
         <v>23</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>22</v>
       </c>
@@ -1138,13 +1455,13 @@
         <v>23</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>22</v>
       </c>
@@ -1152,139 +1469,167 @@
         <v>23</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B34" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>83</v>
+        <v>104</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>24</v>
       </c>
       <c r="B35" t="s">
         <v>25</v>
       </c>
-      <c r="C35" s="2"/>
+      <c r="C35" s="2" t="s">
+        <v>105</v>
+      </c>
       <c r="D35" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>24</v>
       </c>
       <c r="B36" t="s">
         <v>25</v>
       </c>
-      <c r="C36" s="2"/>
+      <c r="C36" s="2" t="s">
+        <v>106</v>
+      </c>
       <c r="D36" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>24</v>
       </c>
       <c r="B37" t="s">
         <v>25</v>
       </c>
+      <c r="C37" t="s">
+        <v>107</v>
+      </c>
       <c r="D37" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B38" t="s">
-        <v>25</v>
+        <v>27</v>
+      </c>
+      <c r="C38" t="s">
+        <v>165</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>26</v>
       </c>
       <c r="B39" t="s">
         <v>27</v>
       </c>
+      <c r="C39" t="s">
+        <v>166</v>
+      </c>
       <c r="D39" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>26</v>
       </c>
       <c r="B40" t="s">
         <v>27</v>
       </c>
+      <c r="C40" t="s">
+        <v>167</v>
+      </c>
       <c r="D40" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>26</v>
       </c>
       <c r="B41" t="s">
         <v>27</v>
       </c>
+      <c r="C41" t="s">
+        <v>168</v>
+      </c>
       <c r="D41" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B42" t="s">
-        <v>27</v>
+        <v>29</v>
+      </c>
+      <c r="C42" t="s">
+        <v>156</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>28</v>
       </c>
       <c r="B43" t="s">
         <v>29</v>
       </c>
+      <c r="C43" t="s">
+        <v>157</v>
+      </c>
       <c r="D43" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>28</v>
       </c>
       <c r="B44" t="s">
         <v>29</v>
       </c>
+      <c r="C44" t="s">
+        <v>158</v>
+      </c>
       <c r="D44" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>28</v>
       </c>
@@ -1295,40 +1640,49 @@
         <v>7</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B46" t="s">
-        <v>29</v>
+        <v>31</v>
+      </c>
+      <c r="C46" t="s">
+        <v>159</v>
       </c>
       <c r="D46" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>30</v>
       </c>
       <c r="B47" t="s">
         <v>31</v>
       </c>
+      <c r="C47" t="s">
+        <v>160</v>
+      </c>
       <c r="D47" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>30</v>
       </c>
       <c r="B48" t="s">
         <v>31</v>
       </c>
+      <c r="C48" t="s">
+        <v>161</v>
+      </c>
       <c r="D48" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>30</v>
       </c>
@@ -1339,73 +1693,91 @@
         <v>7</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B50" t="s">
-        <v>31</v>
+        <v>33</v>
+      </c>
+      <c r="C50" t="s">
+        <v>169</v>
       </c>
       <c r="D50" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>32</v>
       </c>
       <c r="B51" t="s">
         <v>33</v>
       </c>
+      <c r="C51" t="s">
+        <v>170</v>
+      </c>
       <c r="D51" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>32</v>
       </c>
       <c r="B52" t="s">
         <v>33</v>
       </c>
+      <c r="C52" t="s">
+        <v>171</v>
+      </c>
       <c r="D52" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>32</v>
       </c>
       <c r="B53" t="s">
         <v>33</v>
       </c>
+      <c r="C53" t="s">
+        <v>172</v>
+      </c>
       <c r="D53" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B54" t="s">
-        <v>33</v>
+        <v>35</v>
+      </c>
+      <c r="C54" t="s">
+        <v>131</v>
       </c>
       <c r="D54" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>34</v>
       </c>
       <c r="B55" t="s">
         <v>35</v>
       </c>
+      <c r="C55" t="s">
+        <v>132</v>
+      </c>
       <c r="D55" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>34</v>
       </c>
@@ -1416,7 +1788,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>34</v>
       </c>
@@ -1427,40 +1799,49 @@
         <v>7</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B58" t="s">
-        <v>35</v>
+        <v>37</v>
+      </c>
+      <c r="C58" t="s">
+        <v>137</v>
       </c>
       <c r="D58" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>36</v>
       </c>
       <c r="B59" t="s">
         <v>37</v>
       </c>
+      <c r="C59" t="s">
+        <v>138</v>
+      </c>
       <c r="D59" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>36</v>
       </c>
       <c r="B60" t="s">
         <v>37</v>
       </c>
+      <c r="C60" t="s">
+        <v>139</v>
+      </c>
       <c r="D60" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>36</v>
       </c>
@@ -1471,62 +1852,77 @@
         <v>7</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B62" t="s">
-        <v>37</v>
+        <v>39</v>
+      </c>
+      <c r="C62" t="s">
+        <v>133</v>
       </c>
       <c r="D62" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>38</v>
       </c>
       <c r="B63" t="s">
         <v>39</v>
       </c>
+      <c r="C63" t="s">
+        <v>134</v>
+      </c>
       <c r="D63" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>38</v>
       </c>
       <c r="B64" t="s">
         <v>39</v>
       </c>
+      <c r="C64" t="s">
+        <v>135</v>
+      </c>
       <c r="D64" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>38</v>
       </c>
       <c r="B65" t="s">
         <v>39</v>
       </c>
+      <c r="C65" t="s">
+        <v>136</v>
+      </c>
       <c r="D65" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B66" t="s">
-        <v>39</v>
+        <v>41</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>68</v>
       </c>
       <c r="D66" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>40</v>
       </c>
@@ -1534,13 +1930,13 @@
         <v>41</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D67" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>40</v>
       </c>
@@ -1548,13 +1944,13 @@
         <v>41</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D68" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>40</v>
       </c>
@@ -1562,27 +1958,27 @@
         <v>41</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D69" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B70" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>71</v>
+        <v>88</v>
       </c>
       <c r="D70" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>42</v>
       </c>
@@ -1590,13 +1986,13 @@
         <v>43</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D71" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>42</v>
       </c>
@@ -1604,13 +2000,13 @@
         <v>43</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D72" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>42</v>
       </c>
@@ -1618,247 +2014,307 @@
         <v>43</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D73" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B74" t="s">
-        <v>43</v>
-      </c>
-      <c r="C74" s="2" t="s">
-        <v>91</v>
+        <v>45</v>
+      </c>
+      <c r="C74" t="s">
+        <v>152</v>
       </c>
       <c r="D74" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>44</v>
       </c>
       <c r="B75" t="s">
         <v>45</v>
       </c>
+      <c r="C75" t="s">
+        <v>153</v>
+      </c>
       <c r="D75" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>44</v>
       </c>
       <c r="B76" t="s">
         <v>45</v>
       </c>
+      <c r="C76" t="s">
+        <v>154</v>
+      </c>
       <c r="D76" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>44</v>
       </c>
       <c r="B77" t="s">
         <v>45</v>
       </c>
+      <c r="C77" t="s">
+        <v>155</v>
+      </c>
       <c r="D77" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B78" t="s">
-        <v>45</v>
+        <v>47</v>
+      </c>
+      <c r="C78" t="s">
+        <v>121</v>
       </c>
       <c r="D78" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>46</v>
       </c>
       <c r="B79" t="s">
         <v>47</v>
       </c>
+      <c r="C79" t="s">
+        <v>122</v>
+      </c>
       <c r="D79" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>46</v>
       </c>
       <c r="B80" t="s">
         <v>47</v>
       </c>
+      <c r="C80" t="s">
+        <v>120</v>
+      </c>
       <c r="D80" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>46</v>
       </c>
       <c r="B81" t="s">
         <v>47</v>
       </c>
+      <c r="C81" t="s">
+        <v>119</v>
+      </c>
       <c r="D81" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B82" t="s">
-        <v>47</v>
+        <v>49</v>
+      </c>
+      <c r="C82" t="s">
+        <v>123</v>
       </c>
       <c r="D82" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>48</v>
       </c>
       <c r="B83" t="s">
         <v>49</v>
       </c>
+      <c r="C83" t="s">
+        <v>124</v>
+      </c>
       <c r="D83" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>48</v>
       </c>
       <c r="B84" t="s">
         <v>49</v>
       </c>
+      <c r="C84" t="s">
+        <v>125</v>
+      </c>
       <c r="D84" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>48</v>
       </c>
       <c r="B85" t="s">
         <v>49</v>
       </c>
+      <c r="C85" t="s">
+        <v>126</v>
+      </c>
       <c r="D85" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B86" t="s">
-        <v>49</v>
+        <v>51</v>
+      </c>
+      <c r="C86" t="s">
+        <v>127</v>
       </c>
       <c r="D86" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>50</v>
       </c>
       <c r="B87" t="s">
         <v>51</v>
       </c>
+      <c r="C87" t="s">
+        <v>128</v>
+      </c>
       <c r="D87" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>50</v>
       </c>
       <c r="B88" t="s">
         <v>51</v>
       </c>
+      <c r="C88" t="s">
+        <v>129</v>
+      </c>
       <c r="D88" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>50</v>
       </c>
       <c r="B89" t="s">
         <v>51</v>
       </c>
+      <c r="C89" t="s">
+        <v>130</v>
+      </c>
       <c r="D89" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B90" t="s">
-        <v>51</v>
+        <v>53</v>
+      </c>
+      <c r="C90" t="s">
+        <v>173</v>
       </c>
       <c r="D90" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>52</v>
       </c>
       <c r="B91" t="s">
         <v>53</v>
       </c>
+      <c r="C91" t="s">
+        <v>174</v>
+      </c>
       <c r="D91" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>52</v>
       </c>
       <c r="B92" t="s">
         <v>53</v>
       </c>
+      <c r="C92" t="s">
+        <v>175</v>
+      </c>
       <c r="D92" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>52</v>
       </c>
       <c r="B93" t="s">
         <v>53</v>
       </c>
+      <c r="C93" t="s">
+        <v>176</v>
+      </c>
       <c r="D93" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B94" t="s">
-        <v>53</v>
+        <v>55</v>
+      </c>
+      <c r="C94" s="2" t="s">
+        <v>76</v>
       </c>
       <c r="D94" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>54</v>
       </c>
@@ -1866,13 +2322,13 @@
         <v>55</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D95" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>54</v>
       </c>
@@ -1880,13 +2336,13 @@
         <v>55</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D96" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>54</v>
       </c>
@@ -1894,27 +2350,27 @@
         <v>55</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D97" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B98" t="s">
-        <v>55</v>
-      </c>
-      <c r="C98" s="2" t="s">
-        <v>79</v>
+        <v>57</v>
+      </c>
+      <c r="C98" t="s">
+        <v>96</v>
       </c>
       <c r="D98" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>56</v>
       </c>
@@ -1922,13 +2378,13 @@
         <v>57</v>
       </c>
       <c r="C99" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="D99" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>56</v>
       </c>
@@ -1936,13 +2392,13 @@
         <v>57</v>
       </c>
       <c r="C100" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D100" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>56</v>
       </c>
@@ -1950,49 +2406,55 @@
         <v>57</v>
       </c>
       <c r="C101" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D101" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B102" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C102" t="s">
-        <v>98</v>
+        <v>114</v>
       </c>
       <c r="D102" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>58</v>
       </c>
       <c r="B103" t="s">
         <v>59</v>
       </c>
+      <c r="C103" t="s">
+        <v>113</v>
+      </c>
       <c r="D103" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>58</v>
       </c>
       <c r="B104" t="s">
         <v>59</v>
       </c>
+      <c r="C104" t="s">
+        <v>112</v>
+      </c>
       <c r="D104" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>58</v>
       </c>
@@ -2003,18 +2465,21 @@
         <v>7</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B106" t="s">
-        <v>59</v>
+        <v>61</v>
+      </c>
+      <c r="C106" t="s">
+        <v>92</v>
       </c>
       <c r="D106" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>60</v>
       </c>
@@ -2022,13 +2487,13 @@
         <v>61</v>
       </c>
       <c r="C107" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D107" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>60</v>
       </c>
@@ -2036,13 +2501,13 @@
         <v>61</v>
       </c>
       <c r="C108" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D108" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>60</v>
       </c>
@@ -2050,99 +2515,111 @@
         <v>61</v>
       </c>
       <c r="C109" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D109" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B110" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C110" t="s">
-        <v>95</v>
+        <v>108</v>
       </c>
       <c r="D110" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>62</v>
       </c>
       <c r="B111" t="s">
         <v>63</v>
       </c>
+      <c r="C111" t="s">
+        <v>109</v>
+      </c>
       <c r="D111" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>62</v>
       </c>
-      <c r="B112" t="s">
+      <c r="B112" s="3" t="s">
         <v>63</v>
       </c>
+      <c r="C112" t="s">
+        <v>110</v>
+      </c>
       <c r="D112" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>62</v>
       </c>
-      <c r="B113" s="3" t="s">
+      <c r="B113" t="s">
         <v>63</v>
       </c>
+      <c r="C113" t="s">
+        <v>111</v>
+      </c>
       <c r="D113" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B114" t="s">
-        <v>63</v>
+        <v>65</v>
+      </c>
+      <c r="C114" s="2" t="s">
+        <v>84</v>
       </c>
       <c r="D114" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>64</v>
       </c>
       <c r="B115" t="s">
         <v>65</v>
       </c>
-      <c r="C115" s="2" t="s">
-        <v>84</v>
+      <c r="C115" s="4" t="s">
+        <v>87</v>
       </c>
       <c r="D115" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>64</v>
       </c>
       <c r="B116" t="s">
         <v>65</v>
       </c>
-      <c r="C116" s="4" t="s">
-        <v>87</v>
+      <c r="C116" s="2" t="s">
+        <v>85</v>
       </c>
       <c r="D116" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>64</v>
       </c>
@@ -2150,141 +2627,140 @@
         <v>65</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D117" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B118" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>86</v>
+        <v>115</v>
       </c>
       <c r="D118" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>66</v>
       </c>
       <c r="B119" t="s">
         <v>67</v>
       </c>
+      <c r="C119" s="2" t="s">
+        <v>116</v>
+      </c>
       <c r="D119" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>66</v>
       </c>
       <c r="B120" t="s">
         <v>67</v>
       </c>
+      <c r="C120" s="2" t="s">
+        <v>117</v>
+      </c>
       <c r="D120" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>66</v>
       </c>
       <c r="B121" t="s">
         <v>67</v>
       </c>
+      <c r="C121" s="2" t="s">
+        <v>118</v>
+      </c>
       <c r="D121" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A122" t="s">
-        <v>66</v>
-      </c>
-      <c r="B122" t="s">
-        <v>67</v>
-      </c>
-      <c r="D122" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D122" s="2"/>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D123" s="2"/>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D124" s="2"/>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B125" s="3"/>
       <c r="D125" s="2"/>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B126" s="3"/>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D126" s="2"/>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D127" s="2"/>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D128" s="2"/>
     </row>
-    <row r="129" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="129" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D129" s="2"/>
     </row>
-    <row r="130" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="130" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D130" s="2"/>
     </row>
-    <row r="131" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="131" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D131" s="2"/>
     </row>
-    <row r="132" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="132" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D132" s="2"/>
     </row>
-    <row r="133" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="133" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D133" s="2"/>
     </row>
-    <row r="134" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="134" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D134" s="2"/>
     </row>
-    <row r="135" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="135" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D135" s="2"/>
     </row>
-    <row r="136" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="136" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D136" s="2"/>
     </row>
-    <row r="137" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="137" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D137" s="2"/>
     </row>
-    <row r="138" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="138" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D138" s="2"/>
     </row>
-    <row r="139" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="139" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D139" s="2"/>
     </row>
-    <row r="140" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="140" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D140" s="2"/>
     </row>
-    <row r="141" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="141" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D141" s="2"/>
     </row>
-    <row r="142" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="142" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D142" s="2"/>
     </row>
-    <row r="143" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="143" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D143" s="2"/>
     </row>
-    <row r="144" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="144" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D144" s="2"/>
     </row>
-    <row r="145" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D145" s="2"/>
-    </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>